<commit_message>
Updating XS of 13_6 and ta_ta
</commit_message>
<xml_diff>
--- a/01_signal_production/Data_Generation_wRHC/Data_5K_13_6_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
+++ b/01_signal_production/Data_Generation_wRHC/Data_5K_13_6_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1750</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>2250</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>1750</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>2250</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -488,297 +473,1597 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.0625</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1052</v>
+        <v>0.2478</v>
       </c>
       <c r="C2" t="n">
-        <v>23.35</v>
+        <v>0.04371</v>
       </c>
       <c r="D2" t="n">
-        <v>1.846</v>
+        <v>0.008815999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2466</v>
+        <v>0.002016</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04334</v>
+        <v>0.0004901</v>
       </c>
       <c r="G2" t="n">
-        <v>0.008821000000000001</v>
+        <v>0.0001244</v>
       </c>
       <c r="H2" t="n">
-        <v>0.002007</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0004886</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.0001241</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3.269e-05</v>
+        <v>3.242e-05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.125</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1056</v>
+        <v>0.2473</v>
       </c>
       <c r="C3" t="n">
-        <v>23.27</v>
+        <v>0.04324</v>
       </c>
       <c r="D3" t="n">
-        <v>1.844</v>
+        <v>0.008828000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2472</v>
+        <v>0.002011</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04355</v>
+        <v>0.0004897</v>
       </c>
       <c r="G3" t="n">
-        <v>0.008871</v>
+        <v>0.0001245</v>
       </c>
       <c r="H3" t="n">
-        <v>0.002008</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0004892</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.0001243</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3.246e-05</v>
+        <v>3.27e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.1875</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1058</v>
+        <v>0.2459</v>
       </c>
       <c r="C4" t="n">
-        <v>23.28</v>
+        <v>0.04329</v>
       </c>
       <c r="D4" t="n">
-        <v>1.845</v>
+        <v>0.008850999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2471</v>
+        <v>0.002007</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04337</v>
+        <v>0.0004878</v>
       </c>
       <c r="G4" t="n">
-        <v>0.008855</v>
+        <v>0.0001244</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002007</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0004874</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.0001238</v>
-      </c>
-      <c r="K4" t="n">
-        <v>3.261e-05</v>
+        <v>3.256e-05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1059</v>
+        <v>0.2484</v>
       </c>
       <c r="C5" t="n">
-        <v>23.48</v>
+        <v>0.04326</v>
       </c>
       <c r="D5" t="n">
-        <v>1.855</v>
+        <v>0.008836</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2492</v>
+        <v>0.002006</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04347</v>
+        <v>0.0004864</v>
       </c>
       <c r="G5" t="n">
-        <v>0.008872</v>
+        <v>0.0001248</v>
       </c>
       <c r="H5" t="n">
-        <v>0.002019</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0004872</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.000125</v>
-      </c>
-      <c r="K5" t="n">
-        <v>3.261e-05</v>
+        <v>3.247e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.3125</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1071</v>
+        <v>0.2464</v>
       </c>
       <c r="C6" t="n">
-        <v>23.95</v>
+        <v>0.04336</v>
       </c>
       <c r="D6" t="n">
-        <v>1.896</v>
+        <v>0.008848999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2523</v>
+        <v>0.002008</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0441</v>
+        <v>0.0004877</v>
       </c>
       <c r="G6" t="n">
-        <v>0.008985999999999999</v>
+        <v>0.0001239</v>
       </c>
       <c r="H6" t="n">
-        <v>0.002044</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0004979</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.0001257</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3.296e-05</v>
+        <v>3.246e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>0.375</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1094</v>
+        <v>0.2467</v>
       </c>
       <c r="C7" t="n">
-        <v>24.65</v>
+        <v>0.04348</v>
       </c>
       <c r="D7" t="n">
-        <v>1.953</v>
+        <v>0.008876</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2611</v>
+        <v>0.002006</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04571</v>
+        <v>0.0004887</v>
       </c>
       <c r="G7" t="n">
-        <v>0.009202999999999999</v>
+        <v>0.0001241</v>
       </c>
       <c r="H7" t="n">
-        <v>0.002101</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0005077</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.000128</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3.346e-05</v>
+        <v>3.254e-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.4375</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1159</v>
+        <v>0.2478</v>
       </c>
       <c r="C8" t="n">
-        <v>26.07</v>
+        <v>0.04316</v>
       </c>
       <c r="D8" t="n">
-        <v>2.076</v>
+        <v>0.008827</v>
       </c>
       <c r="E8" t="n">
-        <v>0.279</v>
+        <v>0.002017</v>
       </c>
       <c r="F8" t="n">
-        <v>0.04825</v>
+        <v>0.0004872</v>
       </c>
       <c r="G8" t="n">
-        <v>0.009762</v>
+        <v>0.000124</v>
       </c>
       <c r="H8" t="n">
-        <v>0.002213</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0005351000000000001</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.0001337</v>
-      </c>
-      <c r="K8" t="n">
-        <v>3.472e-05</v>
+        <v>3.251e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.2474</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.04342</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.008841</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002011</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0004886</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0001248</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.254e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>0.5625</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.2459</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.04327</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008871</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002004</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0004895</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0001246</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.256e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.2488</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.04332</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.008846</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002009</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0004927</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0001239</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.259e-05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>0.6875</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.2478</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.04352</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.008840000000000001</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.002005</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.000491</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0001241</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3.252e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.2471</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.04346</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.008802000000000001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.002004</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0004909</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0001248</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3.237e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>0.8125</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.2491</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.04338</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.008787</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.002011</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0004903</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0001242</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3.249e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>0.875</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2424</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.04304</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.008852</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.002013</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.000491</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0001243</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3.244e-05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>0.9375</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2468</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.04325</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.008817999999999999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001999</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0004887</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0001244</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3.246e-05</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2483</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.04336</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.008836</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.002003</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0004859</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.000124</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3.285e-05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>1.0625</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.2462</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.04319</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.008836999999999999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.002013</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0004871</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0001237</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3.247e-05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>1.125</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.2476</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.04314</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.008843</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.00201</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0004909</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0001245</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3.245e-05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>1.1875</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.2463</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.04307</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.008857</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.002002</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0004916</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0001244</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3.259e-05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2474</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.04344</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.008826000000000001</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.002013</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0004881</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0001242</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3.271e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>1.3125</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2472</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.04354</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.008827</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.002027</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0004868</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0001244</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3.288e-05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>1.375</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.2468</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.04339</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.008937</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.002011</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.000492</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0001241</v>
+      </c>
+      <c r="H23" t="n">
+        <v>3.262e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>1.4375</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.2489</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.008864</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.002027</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0004882</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0001248</v>
+      </c>
+      <c r="H24" t="n">
+        <v>3.259e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.2464</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0436</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.008865</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.002022</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0004908</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0001257</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3.276e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>1.5625</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.2464</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.04332</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.008836</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.002018</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0004934</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0001249</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3.265e-05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>1.625</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.2463</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.04342</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.008884</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.002007</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0004918</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0001249</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3.291e-05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>1.6875</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.2486</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.04368</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.008917</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.002026</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.0004898</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.0001251</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3.274e-05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.2506</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.04372</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.008881</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.002024</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0004947</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0001264</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3.261e-05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>1.8125</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.2497</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.04403</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.008839</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.002027</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.0004929999999999999</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.0001249</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3.277e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>1.875</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.2527</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.04384</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.008987</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.002028</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0004945</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.0001256</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3.281e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>1.9375</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.2519</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.04395</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.008982</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.002037</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.0004955</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.0001258</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3.278e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.2536</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.04402</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.008921999999999999</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.002049</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.0004951000000000001</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.0001261</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3.292e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>2.0625</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.2542</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0443</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.008961999999999999</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.002051</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.0001261</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3.301e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>2.125</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.04449</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.008996000000000001</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.002056</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0004995000000000001</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0001267</v>
+      </c>
+      <c r="H35" t="n">
+        <v>3.307e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>2.1875</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.2543</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.04474</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.009024000000000001</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.002056</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.0005027</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.0001267</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3.289e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.2552</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.04479</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.009098999999999999</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.002065</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.0005005</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.0001266</v>
+      </c>
+      <c r="H37" t="n">
+        <v>3.313e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>2.3125</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.2571</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.04489</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.009122999999999999</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.002063</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.000501</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.0001274</v>
+      </c>
+      <c r="H38" t="n">
+        <v>3.329e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>2.375</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.2571</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.04485</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.009105</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.002086</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0005066</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0001282</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3.338e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>2.4375</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.2598</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.04552</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.009168000000000001</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.002086</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.0005066</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.0001282</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3.343e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.2618</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.04547</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.009216999999999999</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.002096</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.0005061</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0001288</v>
+      </c>
+      <c r="H41" t="n">
+        <v>3.378e-05</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>2.5625</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.2633</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.04586</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.009306</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.002103</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.0005081</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.0001288</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3.356e-05</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>2.625</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.2638</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.04605</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.009344999999999999</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.002119</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.0005144</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.00013</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3.37e-05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>2.6875</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.2669</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.04674</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.009397000000000001</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.002141</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.0005158</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.0001309</v>
+      </c>
+      <c r="H44" t="n">
+        <v>3.413e-05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.2663</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.04671</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.009436</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.002139</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.0005215</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.0001311</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3.409e-05</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>2.8125</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.2713</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.04671</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.009512</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.002147</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.0005215</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.0001311</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3.408e-05</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>2.875</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.2716</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0476</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.009636</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.002187</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.0005267</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.0001313</v>
+      </c>
+      <c r="H47" t="n">
+        <v>3.438e-05</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>2.9375</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.2765</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.04814</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.009665999999999999</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.002192</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.0005299</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.0001327</v>
+      </c>
+      <c r="H48" t="n">
+        <v>3.449e-05</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.2792</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.04804</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.009714</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.002194</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.0005337</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.0001337</v>
+      </c>
+      <c r="H49" t="n">
+        <v>3.478e-05</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>3.0625</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.2798</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.04891</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.009860000000000001</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.002226</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.0005338</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.0001347</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3.506e-05</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>3.125</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.2824</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.04888</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.009953999999999999</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.002239</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.0005411</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.0001357</v>
+      </c>
+      <c r="H51" t="n">
+        <v>3.508e-05</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>3.1875</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.2887</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.04978</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.01006</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.002273</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.0005442999999999999</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.0001367</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3.541e-05</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.2896</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.05012</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01017</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.00229</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.0005477</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.0001379</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3.561e-05</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>3.3125</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.2928</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.05038</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01023</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.00231</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.0005579</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.0001388</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3.561e-05</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>3.375</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.2974</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0519</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.01035</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.002341</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0005637</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.00014</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3.602e-05</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>3.4375</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0521</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.01047</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.002355</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.0005683</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.000142</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3.622e-05</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
           <t>3.5</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1256</v>
-      </c>
-      <c r="C9" t="n">
-        <v>28.72</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2.304</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.3047</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0527</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.01061</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.002388</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0005724</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.0001431</v>
-      </c>
-      <c r="K9" t="n">
-        <v>3.658e-05</v>
+      <c r="B57" t="n">
+        <v>0.3058</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.05287</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.01064</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.002399</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.000577</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.0001425</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3.67e-05</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.2503</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.04389</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.008879</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.002025</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0004934</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.0001256</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3.273e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>